<commit_message>
we have IRF with SVAR
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Aussie\Monash\Macroeconometrics\Replicate\MillikenRepGali1999\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC5BF8B-95BA-4447-9BD5-F6CC710EC7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED2979A-1AB2-4F68-942D-7B6F3536086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
   <si>
     <t>GDPQ</t>
   </si>
@@ -665,6 +665,9 @@
   </si>
   <si>
     <t>NBERG</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1018,6 +1021,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>

</xml_diff>